<commit_message>
SISTEMI - ufficio ceo
</commit_message>
<xml_diff>
--- a/altro/sistemiReti/Subnetting_azienda.xlsx
+++ b/altro/sistemiReti/Subnetting_azienda.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\repositoryElaborato\altro\sistemiReti\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB5DE3BD-ABA0-4EC7-B0EB-8E15D37487E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB52F18A-F0A6-46CE-85B0-167D7373B0BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{73B77B31-CD31-478B-AB0E-C19DC6E5E5D6}"/>
   </bookViews>
@@ -45,9 +45,6 @@
     <t>BROADCAST</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
     <t>TOT</t>
   </si>
   <si>
@@ -197,7 +194,10 @@
     <t>192.168.1.14</t>
   </si>
   <si>
-    <t>SUBNETTING RETE DI CLASSE C (Area Server Room)</t>
+    <t>Server Room</t>
+  </si>
+  <si>
+    <t>SUBNETTING RETE DI CLASSE C</t>
   </si>
 </sst>
 </file>
@@ -670,7 +670,7 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -694,7 +694,7 @@
     </row>
     <row r="2" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -726,15 +726,15 @@
         <v>5</v>
       </c>
       <c r="H3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="B4" s="1">
         <v>12</v>
@@ -750,13 +750,13 @@
         <v>28</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="I4" s="5">
         <v>255255255240</v>
@@ -764,7 +764,7 @@
     </row>
     <row r="5" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1">
         <f>SUM(B4)</f>
@@ -786,28 +786,28 @@
     </row>
     <row r="10" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="D10" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="E10" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="F10" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="G10" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="H10" s="9" t="s">
         <v>17</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>